<commit_message>
commit con recomendaciones y readme
</commit_message>
<xml_diff>
--- a/Diccionario de Datos STEAM.xlsx
+++ b/Diccionario de Datos STEAM.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5b9be641770c559e/Escritorio/William/proyecto_individual/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_B47BD9647E544E6EBB2B5625015ACAC102BE439A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7DD95FD9-D3EF-4AAD-B35B-1E2A130504D9}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -205,44 +214,51 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -252,41 +268,54 @@
     </fill>
   </fills>
   <borders count="5">
-    <border/>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -296,52 +325,51 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+  <cellXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -531,308 +559,315 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="11.75"/>
-    <col customWidth="1" min="2" max="2" width="27.13"/>
-    <col customWidth="1" min="3" max="3" width="80.13"/>
+    <col min="1" max="1" width="11.77734375" customWidth="1"/>
+    <col min="2" max="2" width="27.109375" customWidth="1"/>
+    <col min="3" max="3" width="88.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="5" t="s">
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="7"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="2" t="s">
+      <c r="B19" s="9"/>
+      <c r="C19" s="10"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="8"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="3" t="s">
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="3" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="9"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="5" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="7"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="2" t="s">
+      <c r="B25" s="9"/>
+      <c r="C25" s="10"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="3" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="3" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="2" t="s">
         <v>62</v>
       </c>
     </row>
@@ -843,11 +878,11 @@
     <mergeCell ref="A25:C25"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="C7"/>
-    <hyperlink r:id="rId2" ref="C11"/>
-    <hyperlink r:id="rId3" ref="C22"/>
-    <hyperlink r:id="rId4" ref="C28"/>
+    <hyperlink ref="C7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C11" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C22" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C28" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
-  <drawing r:id="rId5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>